<commit_message>
Bringing data back to normal
</commit_message>
<xml_diff>
--- a/data/sizes/B_2023POGS_small_seed_daily/B_sizes_12172024.xlsx
+++ b/data/sizes/B_2023POGS_small_seed_daily/B_sizes_12172024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graceleuchtenberger/Library/Mobile Documents/com~apple~CloudDocs/Documents/project-gigas-conditioning-GL/data/sizes/B_2023POGS_small_seed_daily/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BDF2399-C783-A545-865F-4D971B164C1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E494A7-5341-304F-BCB6-73133A5B4AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10460" yWindow="740" windowWidth="19020" windowHeight="17160" xr2:uid="{59562AC7-2699-D84F-A30D-CDAA438C0A0D}"/>
+    <workbookView xWindow="4640" yWindow="740" windowWidth="24840" windowHeight="17160" xr2:uid="{59562AC7-2699-D84F-A30D-CDAA438C0A0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -516,9 +516,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{951AA300-CB28-DA47-A4F6-6DBA5477955B}">
   <dimension ref="A1:XFD711"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="163" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A602" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N701" sqref="N701:N711"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="163" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A604" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I612" sqref="I612"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>